<commit_message>
minor comments added to supp tables
</commit_message>
<xml_diff>
--- a/Manuscript/Revision/TableS2.xlsx
+++ b/Manuscript/Revision/TableS2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37540" yWindow="-2160" windowWidth="35820" windowHeight="18160" tabRatio="500"/>
+    <workbookView xWindow="-36220" yWindow="-1020" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="147">
   <si>
     <t>HA</t>
   </si>
@@ -457,6 +457,9 @@
   </si>
   <si>
     <t>0.2931 (-3.53%)***</t>
+  </si>
+  <si>
+    <t>Caption for table essentially same as Table 1 in main text.</t>
   </si>
 </sst>
 </file>
@@ -513,8 +516,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -557,9 +580,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -578,8 +598,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -597,6 +620,16 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -614,6 +647,16 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -943,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3:V16"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -968,26 +1011,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
@@ -1049,220 +1092,220 @@
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>8.43E-2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="7">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>8.6199999999999999E-2</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>8.1600000000000006E-2</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="7">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="7">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>26</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.25180000000000002</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.2273</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="7">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <v>1.9E-3</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>26</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.2092</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.17549999999999999</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>44</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1274,59 +1317,59 @@
       <c r="K6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="7">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="Q6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="R6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="S6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>60</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.55130000000000001</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.47399999999999998</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>36</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1338,114 +1381,114 @@
       <c r="K7" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="7">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R7" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="S7" s="4" t="s">
+      <c r="S7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>60</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.4219</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.34739999999999999</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="7">
         <v>1E-4</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="8">
         <v>2.8E-3</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="P8" s="10" t="s">
+      <c r="P8" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="Q8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="R8" s="10" t="s">
+      <c r="R8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="S8" s="10" t="s">
+      <c r="S8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>158</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.51519999999999999</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.45810000000000001</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1466,114 +1509,114 @@
       <c r="K9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="S9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>6.2300000000000001E-2</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="7">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="7">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="O10" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="Q10" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="R10" s="10" t="s">
+      <c r="R10" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="S10" s="10" t="s">
+      <c r="S10" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>11</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>9.5899999999999999E-2</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>9.8199999999999996E-2</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1594,50 +1637,50 @@
       <c r="K11" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <v>1.8E-3</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>3.3E-3</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="P11" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="Q11" s="10" t="s">
+      <c r="Q11" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="R11" s="10" t="s">
+      <c r="R11" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="S11" s="10" t="s">
+      <c r="S11" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>26</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>0.21560000000000001</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.1963</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1649,196 +1692,196 @@
       <c r="H12" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="6">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N12" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="O12" s="13" t="s">
+      <c r="O12" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="P12" s="13" t="s">
+      <c r="P12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="Q12" s="10" t="s">
+      <c r="Q12" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="R12" s="10" t="s">
+      <c r="R12" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="S12" s="10" t="s">
+      <c r="S12" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>0.23680000000000001</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>0.21629999999999999</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>64</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="6">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <v>4.3E-3</v>
       </c>
-      <c r="N13" s="13" t="s">
+      <c r="N13" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="O13" s="13" t="s">
+      <c r="O13" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="Q13" s="10" t="s">
+      <c r="Q13" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="R13" s="10" t="s">
+      <c r="R13" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="S13" s="10" t="s">
+      <c r="S13" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>60</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>0.3594</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>0.3075</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J14" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="6">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="6">
         <v>1.09E-2</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="N14" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="O14" s="10" t="s">
+      <c r="O14" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="P14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="Q14" s="10" t="s">
+      <c r="Q14" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="R14" s="10" t="s">
+      <c r="R14" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="S14" s="10" t="s">
+      <c r="S14" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>60</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>0.34129999999999999</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>0.30380000000000001</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -1850,50 +1893,50 @@
       <c r="K15" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="7">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="6">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="N15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Q15" s="4" t="s">
+      <c r="Q15" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="S15" s="4" t="s">
+      <c r="S15" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>158</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>0.34379999999999999</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>0.31950000000000001</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -1914,63 +1957,195 @@
       <c r="K16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="7">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16" s="7">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="N16" s="10" t="s">
+      <c r="N16" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="P16" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="Q16" s="10" t="s">
+      <c r="Q16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="R16" s="10" t="s">
+      <c r="R16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="S16" s="10" t="s">
+      <c r="S16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="6" t="s">
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="6" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="9"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>